<commit_message>
Programa seircovid_rd y datos por provincias
</commit_message>
<xml_diff>
--- a/datos_salud_publica.xlsx
+++ b/datos_salud_publica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215D21E5-34A7-41F0-B9DF-BA9E87DB33D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92FD7BF-BC8A-45C7-BF21-2BDD1940C34C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3594670B-8219-4C56-B1A5-969C2FE02038}"/>
   </bookViews>
@@ -28,6 +28,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>data</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,86 +385,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF61A583-01C3-4D94-ACD4-951BEA2F9A4B}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>112</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>202</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>245</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>312</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>392</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>488</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>581</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>719</v>
+        <v>581</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>859</v>
       </c>
     </row>

</xml_diff>